<commit_message>
Updated Excel report with new expected values
</commit_message>
<xml_diff>
--- a/deliverables/CPA_Report_Group24.xlsx
+++ b/deliverables/CPA_Report_Group24.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/almax/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/almax/Documents/NTNU/23h/marketing/eth-marketing23/deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0A5EC4B-F7D2-F24A-B51D-6C3CABBF0995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F36986-E9C4-7F42-B951-83C340BE8D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="3280" windowWidth="35640" windowHeight="13300" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1540" yWindow="800" windowWidth="32600" windowHeight="17500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="group" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="194">
   <si>
     <t>group_id</t>
   </si>
@@ -468,57 +468,6 @@
     <t>0.56530</t>
   </si>
   <si>
-    <t>5.29201</t>
-  </si>
-  <si>
-    <t>2.27332</t>
-  </si>
-  <si>
-    <t>0.31956</t>
-  </si>
-  <si>
-    <t>0.18065</t>
-  </si>
-  <si>
-    <t>0.10212</t>
-  </si>
-  <si>
-    <t>0.05773</t>
-  </si>
-  <si>
-    <t>0.03263</t>
-  </si>
-  <si>
-    <t>0.01845</t>
-  </si>
-  <si>
-    <t>0.01043</t>
-  </si>
-  <si>
-    <t>0.00590</t>
-  </si>
-  <si>
-    <t>0.00333</t>
-  </si>
-  <si>
-    <t>0.00188</t>
-  </si>
-  <si>
-    <t>0.05753</t>
-  </si>
-  <si>
-    <t>0.01415</t>
-  </si>
-  <si>
-    <t>0.00602</t>
-  </si>
-  <si>
-    <t>0.00027</t>
-  </si>
-  <si>
-    <t>0.00016</t>
-  </si>
-  <si>
     <t>0.00005</t>
   </si>
   <si>
@@ -561,12 +510,6 @@
     <t>12.69215</t>
   </si>
   <si>
-    <t>23.75619</t>
-  </si>
-  <si>
-    <t>126922.11656</t>
-  </si>
-  <si>
     <t>0.46000</t>
   </si>
   <si>
@@ -636,9 +579,6 @@
     <t>0.89835</t>
   </si>
   <si>
-    <t>16.05373</t>
-  </si>
-  <si>
     <t>0.28571</t>
   </si>
   <si>
@@ -652,6 +592,45 @@
   </si>
   <si>
     <t>0.23178</t>
+  </si>
+  <si>
+    <t>2.30044</t>
+  </si>
+  <si>
+    <t>1.50568</t>
+  </si>
+  <si>
+    <t>0.03194</t>
+  </si>
+  <si>
+    <t>0.00571</t>
+  </si>
+  <si>
+    <t>0.00102</t>
+  </si>
+  <si>
+    <t>0.00018</t>
+  </si>
+  <si>
+    <t>0.00001</t>
+  </si>
+  <si>
+    <t>0.03409</t>
+  </si>
+  <si>
+    <t>0.01010</t>
+  </si>
+  <si>
+    <t>0.00631</t>
+  </si>
+  <si>
+    <t>15.67312</t>
+  </si>
+  <si>
+    <t>126921.50708</t>
+  </si>
+  <si>
+    <t>15.83498</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1112,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1141,7 +1120,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1149,7 +1128,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1157,7 +1136,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1165,7 +1144,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1173,7 +1152,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1181,7 +1160,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1189,7 +1168,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1197,7 +1176,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1205,7 +1184,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1213,7 +1192,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1221,7 +1200,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1229,7 +1208,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1237,7 +1216,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1245,7 +1224,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1253,7 +1232,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1261,7 +1240,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1269,7 +1248,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1277,7 +1256,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1285,7 +1264,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1293,7 +1272,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1301,7 +1280,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1309,7 +1288,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1322,8 +1301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1336,7 +1315,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -1419,7 +1398,7 @@
         <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1427,7 +1406,7 @@
         <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1480,7 +1459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1499,7 +1478,7 @@
         <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1507,7 +1486,7 @@
         <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1515,7 +1494,7 @@
         <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2244,7 +2223,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2259,10 +2238,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>140</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2276,7 +2255,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2308,10 +2287,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>138</v>
+        <v>81</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>131</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2319,10 +2298,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>141</v>
+        <v>183</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2330,10 +2309,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>142</v>
+        <v>184</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2341,10 +2320,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2352,10 +2331,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>154</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2363,10 +2342,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>155</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2374,10 +2353,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>146</v>
+        <v>187</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>156</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2385,10 +2364,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>147</v>
+        <v>80</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>156</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2396,10 +2375,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>148</v>
+        <v>80</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>156</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2407,10 +2386,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>149</v>
+        <v>80</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>156</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2418,7 +2397,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>75</v>
@@ -2453,7 +2432,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2461,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2469,7 +2448,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2477,7 +2456,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2485,7 +2464,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2493,7 +2472,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2501,7 +2480,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2509,7 +2488,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -2517,7 +2496,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -2525,7 +2504,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -2533,7 +2512,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -2541,7 +2520,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2555,7 +2534,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2570,10 +2549,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2587,7 +2566,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2599,7 +2578,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>